<commit_message>
Componets list for S3 dsp board
</commit_message>
<xml_diff>
--- a/pcb/ESP-32-DSP_board/Components.xlsx
+++ b/pcb/ESP-32-DSP_board/Components.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markuslang/Desktop/suunnattava-suuntamikrofoni/pcb/ESP-32-DSP_board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E2252-9AAE-F24A-B138-2825198D7635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58352E3D-91F2-CA4E-AEB7-723BF22AC10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="16720" windowHeight="24200" xr2:uid="{9259DFBC-D495-B44E-BE0B-197FFC43B4CA}"/>
+    <workbookView xWindow="1620" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{9259DFBC-D495-B44E-BE0B-197FFC43B4CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="bom" localSheetId="0">Sheet1!$A$1:$D$37</definedName>
+    <definedName name="bom" localSheetId="0">Sheet1!$A$1:$D$35</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
   <si>
     <t>Designator</t>
   </si>
@@ -78,9 +78,6 @@
     <t>10u</t>
   </si>
   <si>
-    <t>C11, C12, C14, C15, C3, C31, C32, C36, C4, C6</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -114,12 +111,6 @@
     <t>C33, C34</t>
   </si>
   <si>
-    <t>12p</t>
-  </si>
-  <si>
-    <t>C37, C9</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -261,15 +252,6 @@
     <t>Boot</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8</t>
-  </si>
-  <si>
-    <t>TestPoint_Pad_D1.0mm</t>
-  </si>
-  <si>
-    <t>TestPoint</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -339,10 +321,55 @@
     <t>https://www.digikey.fi/fi/products/detail/murata-electronics/GRM188R61A106ME69D/5027560</t>
   </si>
   <si>
-    <t>Cost / unit</t>
-  </si>
-  <si>
     <t>https://www.digikey.fi/fi/products/detail/samsung-electro-mechanics/CL05A104KA5NNNC/3886701</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/samsung-electro-mechanics/CL10A475KP8NNNC/3886702</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/texas-instruments/ADS8688AIDBT/5417855</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/ecs-inc/ECS-400-18-33-JGN-TR3/14825140</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/texas-instruments/LM386MX-1-NOPB/212680</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/stmicroelectronics/USBLC6-2P6/1007440?s=N4IgTCBcDaIKoGUBCAZAwgNgLRgAoZAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/analog-devices-inc/AD5689BRUZ/3925735</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672?s=N4IgTCBcDaIIIC0CMKDsBJAEgWgMwDpcQBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.mouser.fi/ProductDetail/Espressif-Systems/ESP32-S3FH4R2?qs=tlsG%2FOw5FFjPrwkmZSBQNA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/alps-alpine/SKRKAHE020/19529210</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/kycon-inc/STX-3500-3NTR/9975996</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/kemet/C0805C224K5RAC7800/754753</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/tdk-corporation/C1005C0G1H102J050BE/11697944?s=N4IgTCBcDaIMIEMAOCDGBLALgewE4AIBGAO3wBYAGCAXQF8g</t>
+  </si>
+  <si>
+    <t>Cost / unit [€]</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/johanson-technology-inc/QSCF500Q3R3B1GV001T/1561531</t>
+  </si>
+  <si>
+    <t>12p (C-CRYSTAL)(</t>
+  </si>
+  <si>
+    <t>C11, C12, C14, C15, C3, C31, C32, C36, C4, C6, C37, C9</t>
   </si>
 </sst>
 </file>
@@ -709,20 +736,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789DDA5E-B843-9F4D-A7DD-BCDEC96146DF}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="183" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="97.83203125" customWidth="1"/>
+    <col min="6" max="6" width="144.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -739,10 +766,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -762,32 +789,32 @@
         <v>0.12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="B3">
         <v>402</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>0.09</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>603</v>
@@ -796,12 +823,18 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0.09</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>603</v>
@@ -810,12 +843,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>805</v>
@@ -826,10 +860,16 @@
       <c r="D6" t="s">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>0.12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>402</v>
@@ -838,12 +878,18 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>0.18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>402</v>
@@ -852,12 +898,18 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>0.24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>402</v>
@@ -866,46 +918,46 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10">
-        <v>603</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>805</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
-        <v>805</v>
-      </c>
       <c r="C12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -919,7 +971,7 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -961,13 +1013,13 @@
         <v>36</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -975,13 +1027,13 @@
         <v>39</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -994,8 +1046,14 @@
       <c r="D18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>1.5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1009,138 +1067,150 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20">
+        <v>603</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
         <v>48</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>402</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
         <v>50</v>
       </c>
-      <c r="B21">
-        <v>603</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>805</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>402</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>54</v>
-      </c>
-      <c r="B23">
-        <v>805</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>55</v>
       </c>
       <c r="B24">
         <v>402</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>57</v>
       </c>
       <c r="B25">
         <v>402</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>59</v>
-      </c>
-      <c r="B26">
-        <v>402</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>62</v>
       </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>0.72</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
       <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
         <v>64</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28">
+        <v>0.72</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1148,8 +1218,14 @@
       <c r="D29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0.36</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -1157,13 +1233,19 @@
         <v>69</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>10.66</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -1176,8 +1258,14 @@
       <c r="D31" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>0.59</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -1190,8 +1278,14 @@
       <c r="D32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>1.05</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1204,8 +1298,14 @@
       <c r="D33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>19.29</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -1218,8 +1318,14 @@
       <c r="D34" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>2.16</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -1232,32 +1338,10 @@
       <c r="D35" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E35">
+        <v>0.4</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1265,6 +1349,18 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{A0BC24F9-C8CF-D642-BBB5-ED61ECF9C772}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{248AA165-6196-3241-92E7-80EEA7B9F937}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{1235C457-0442-4C40-9E25-2232988DAC63}"/>
+    <hyperlink ref="F33" r:id="rId4" xr:uid="{5FB7B0C0-9104-0D4F-BAC9-F72E611D68BB}"/>
+    <hyperlink ref="F32" r:id="rId5" xr:uid="{04831F98-6843-3B4D-9A8A-DF8BDE60A9AA}"/>
+    <hyperlink ref="F31" r:id="rId6" xr:uid="{913EDCA8-2D49-C14B-928E-896890F133E1}"/>
+    <hyperlink ref="F35" r:id="rId7" xr:uid="{B6BC4450-CDCA-0649-98B4-16A72C06A4F9}"/>
+    <hyperlink ref="F30" r:id="rId8" xr:uid="{192F63ED-5719-7F48-8965-63E72A9B9854}"/>
+    <hyperlink ref="F34" r:id="rId9" xr:uid="{F6CE2FAF-1544-A54A-BB92-0E61A7F4B6DE}"/>
+    <hyperlink ref="F27" r:id="rId10" xr:uid="{E2B175DE-1272-9148-BA26-6AEB71D8F469}"/>
+    <hyperlink ref="F28" r:id="rId11" xr:uid="{F253677C-6697-FB4D-97BF-9492DFC552FD}"/>
+    <hyperlink ref="F29" r:id="rId12" xr:uid="{D1B486A4-4A98-2846-89D2-9F96A342C066}"/>
+    <hyperlink ref="F6" r:id="rId13" xr:uid="{75E55B66-2BA9-4349-A6AE-DBD50C6039FB}"/>
+    <hyperlink ref="F7" r:id="rId14" xr:uid="{D7C81AFD-3ADF-904B-BBF8-68F06FD3303A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added all component order links
</commit_message>
<xml_diff>
--- a/pcb/ESP-32-DSP_board/Components.xlsx
+++ b/pcb/ESP-32-DSP_board/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markuslang/Desktop/suunnattava-suuntamikrofoni/pcb/ESP-32-DSP_board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58352E3D-91F2-CA4E-AEB7-723BF22AC10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A5F90-FE88-7F40-B489-BAE0378968BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{9259DFBC-D495-B44E-BE0B-197FFC43B4CA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="bom" localSheetId="0">Sheet1!$A$1:$D$35</definedName>
+    <definedName name="bom" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>Designator</t>
   </si>
@@ -111,30 +111,12 @@
     <t>C33, C34</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>CP_Radial_D5.0mm_P2.50mm</t>
-  </si>
-  <si>
-    <t>250u</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
     <t>LED</t>
   </si>
   <si>
-    <t>H1, H2, H3, H4</t>
-  </si>
-  <si>
-    <t>MountingHole_2.2mm_M2_DIN965_Pad</t>
-  </si>
-  <si>
-    <t>MountingHole</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -144,33 +126,6 @@
     <t>USB_C_Receptacle_USB2.0</t>
   </si>
   <si>
-    <t>J12</t>
-  </si>
-  <si>
-    <t>Texas_SWRA117D_2.4GHz_Right</t>
-  </si>
-  <si>
-    <t>Conn_Coaxial</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>PinHeader_1x10_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Conn_01x10_Pin</t>
-  </si>
-  <si>
-    <t>J4, J6, J7</t>
-  </si>
-  <si>
-    <t>PinHeader_1x08_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Conn_01x08_Pin</t>
-  </si>
-  <si>
     <t>J5</t>
   </si>
   <si>
@@ -189,15 +144,6 @@
     <t>AudioJack3</t>
   </si>
   <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>SolderJumper-2_P1.3mm_Bridged_RoundedPad1.0x1.5mm</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Bridged</t>
-  </si>
-  <si>
     <t>L1, L2, L4</t>
   </si>
   <si>
@@ -366,10 +312,46 @@
     <t>https://www.digikey.fi/fi/products/detail/johanson-technology-inc/QSCF500Q3R3B1GV001T/1561531</t>
   </si>
   <si>
-    <t>12p (C-CRYSTAL)(</t>
-  </si>
-  <si>
     <t>C11, C12, C14, C15, C3, C31, C32, C36, C4, C6, C37, C9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/liteon/LTST-C171GKT/386793</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/amphenol-cs-commercial-products/12402012E212A/13683192</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/hirose-electric-co-ltd/DM3D-SF/1786510</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/bourns-inc/3314J-1-103E/86580</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/yageo/RC0402FR-074K7L/2827563</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/yageo/RC0402FR-135K1L/14286364</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/yageo/RC0402FR-071KL/726513</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/panasonic-electronic-components/ERJ-6ENF10R0V/110893</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/bourns-inc/CR0402-FX-1002GLF/3593192</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/johanson-technology-inc/LRC0603CS2N2GV001T/1561288</t>
+  </si>
+  <si>
+    <t>20p (crystal load capacitance)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/murata-electronics/GJM1555C1H200FB01D/2592908</t>
+  </si>
+  <si>
+    <t>https://www.digikey.fi/fi/products/detail/samsung-electro-mechanics/CL10A105KA8NNNC/3886760</t>
   </si>
 </sst>
 </file>
@@ -736,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789DDA5E-B843-9F4D-A7DD-BCDEC96146DF}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,7 +729,7 @@
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="144.1640625" customWidth="1"/>
   </cols>
@@ -766,10 +748,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -789,12 +771,12 @@
         <v>0.12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>402</v>
@@ -809,7 +791,7 @@
         <v>0.09</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -829,7 +811,7 @@
         <v>0.09</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -845,7 +827,12 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="E5">
+        <v>0.09</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -864,7 +851,7 @@
         <v>0.12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -884,7 +871,7 @@
         <v>0.18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -903,8 +890,8 @@
       <c r="E8">
         <v>0.24</v>
       </c>
-      <c r="F8" t="s">
-        <v>102</v>
+      <c r="F8" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -918,35 +905,53 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="E9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>805</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
+      <c r="E10">
+        <v>0.24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11">
-        <v>805</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
+      </c>
+      <c r="E11">
+        <v>0.94</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -957,10 +962,16 @@
         <v>24</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
+      </c>
+      <c r="E12">
+        <v>1.66</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -976,221 +987,299 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
+      <c r="E13">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>603</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
+      <c r="E14">
+        <v>0.09</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>402</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
+      <c r="E15">
+        <v>0.09</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>805</v>
       </c>
       <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>402</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <v>0.09</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>402</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <v>1.5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>98</v>
+        <v>0.09</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>402</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>0.09</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20">
-        <v>603</v>
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>1.73</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21">
-        <v>402</v>
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="E21">
+        <v>0.72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22">
-        <v>805</v>
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22">
-        <v>10</v>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22">
+        <v>0.72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23">
-        <v>402</v>
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="E23">
+        <v>0.36</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24">
-        <v>402</v>
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>10.66</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25">
-        <v>402</v>
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="E25">
+        <v>0.59</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>50</v>
+      <c r="E26">
+        <v>1.05</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>61</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>62</v>
-      </c>
       <c r="E27">
-        <v>0.72</v>
+        <v>19.29</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
         <v>63</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1199,10 +1288,10 @@
         <v>64</v>
       </c>
       <c r="E28">
-        <v>0.72</v>
+        <v>2.16</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1219,130 +1308,10 @@
         <v>67</v>
       </c>
       <c r="E29">
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30">
-        <v>10.66</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
         <v>73</v>
-      </c>
-      <c r="E31">
-        <v>0.59</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32">
-        <v>1.05</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33">
-        <v>19.29</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34">
-        <v>2.16</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35">
-        <v>0.4</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1350,17 +1319,30 @@
     <hyperlink ref="F2" r:id="rId1" xr:uid="{A0BC24F9-C8CF-D642-BBB5-ED61ECF9C772}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{248AA165-6196-3241-92E7-80EEA7B9F937}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{1235C457-0442-4C40-9E25-2232988DAC63}"/>
-    <hyperlink ref="F33" r:id="rId4" xr:uid="{5FB7B0C0-9104-0D4F-BAC9-F72E611D68BB}"/>
-    <hyperlink ref="F32" r:id="rId5" xr:uid="{04831F98-6843-3B4D-9A8A-DF8BDE60A9AA}"/>
-    <hyperlink ref="F31" r:id="rId6" xr:uid="{913EDCA8-2D49-C14B-928E-896890F133E1}"/>
-    <hyperlink ref="F35" r:id="rId7" xr:uid="{B6BC4450-CDCA-0649-98B4-16A72C06A4F9}"/>
-    <hyperlink ref="F30" r:id="rId8" xr:uid="{192F63ED-5719-7F48-8965-63E72A9B9854}"/>
-    <hyperlink ref="F34" r:id="rId9" xr:uid="{F6CE2FAF-1544-A54A-BB92-0E61A7F4B6DE}"/>
-    <hyperlink ref="F27" r:id="rId10" xr:uid="{E2B175DE-1272-9148-BA26-6AEB71D8F469}"/>
-    <hyperlink ref="F28" r:id="rId11" xr:uid="{F253677C-6697-FB4D-97BF-9492DFC552FD}"/>
-    <hyperlink ref="F29" r:id="rId12" xr:uid="{D1B486A4-4A98-2846-89D2-9F96A342C066}"/>
+    <hyperlink ref="F27" r:id="rId4" xr:uid="{5FB7B0C0-9104-0D4F-BAC9-F72E611D68BB}"/>
+    <hyperlink ref="F26" r:id="rId5" xr:uid="{04831F98-6843-3B4D-9A8A-DF8BDE60A9AA}"/>
+    <hyperlink ref="F25" r:id="rId6" xr:uid="{913EDCA8-2D49-C14B-928E-896890F133E1}"/>
+    <hyperlink ref="F29" r:id="rId7" xr:uid="{B6BC4450-CDCA-0649-98B4-16A72C06A4F9}"/>
+    <hyperlink ref="F24" r:id="rId8" xr:uid="{192F63ED-5719-7F48-8965-63E72A9B9854}"/>
+    <hyperlink ref="F28" r:id="rId9" xr:uid="{F6CE2FAF-1544-A54A-BB92-0E61A7F4B6DE}"/>
+    <hyperlink ref="F21" r:id="rId10" xr:uid="{E2B175DE-1272-9148-BA26-6AEB71D8F469}"/>
+    <hyperlink ref="F22" r:id="rId11" xr:uid="{F253677C-6697-FB4D-97BF-9492DFC552FD}"/>
+    <hyperlink ref="F23" r:id="rId12" xr:uid="{D1B486A4-4A98-2846-89D2-9F96A342C066}"/>
     <hyperlink ref="F6" r:id="rId13" xr:uid="{75E55B66-2BA9-4349-A6AE-DBD50C6039FB}"/>
     <hyperlink ref="F7" r:id="rId14" xr:uid="{D7C81AFD-3ADF-904B-BBF8-68F06FD3303A}"/>
+    <hyperlink ref="F8" r:id="rId15" xr:uid="{31A139A0-677C-1744-BBD1-C570D34BD88E}"/>
+    <hyperlink ref="F10" r:id="rId16" xr:uid="{9ECCEB36-1A79-C04D-8E95-B89E97126BF7}"/>
+    <hyperlink ref="F11" r:id="rId17" xr:uid="{A4F3F6E8-CAEB-6940-A3A3-AB9526B6E217}"/>
+    <hyperlink ref="F13" r:id="rId18" xr:uid="{E8AED584-9A67-0841-9279-27CF13062E41}"/>
+    <hyperlink ref="F12" r:id="rId19" xr:uid="{22F107C5-7071-A44D-8E74-628872377B75}"/>
+    <hyperlink ref="F20" r:id="rId20" xr:uid="{BE712889-3286-1648-93EE-3090F82A2EA9}"/>
+    <hyperlink ref="F18" r:id="rId21" xr:uid="{A28BF683-2694-AC47-9CC1-E4D33AEE6DA7}"/>
+    <hyperlink ref="F19" r:id="rId22" xr:uid="{FDB205A5-DF71-0949-AC74-C679FF36E87D}"/>
+    <hyperlink ref="F16" r:id="rId23" xr:uid="{7208EA22-F7F2-B245-88EB-C576787E1481}"/>
+    <hyperlink ref="F17" r:id="rId24" xr:uid="{D5BEADBB-C796-B242-9D43-1F26C9BDC79B}"/>
+    <hyperlink ref="F15" r:id="rId25" xr:uid="{AD3B7C29-B378-9449-A9D2-80AF71952DB5}"/>
+    <hyperlink ref="F9" r:id="rId26" xr:uid="{1F447ECB-06E2-984C-AA8F-C7B21F9D046B}"/>
+    <hyperlink ref="F14" r:id="rId27" xr:uid="{935B0050-284A-0848-9134-49A229FCB193}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added price to components lists
</commit_message>
<xml_diff>
--- a/pcb/ESP-32-DSP_board/Components.xlsx
+++ b/pcb/ESP-32-DSP_board/Components.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markuslang/Desktop/suunnattava-suuntamikrofoni/pcb/ESP-32-DSP_board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A5F90-FE88-7F40-B489-BAE0378968BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E65B5FF-D128-B848-94BB-FD428F4F1925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{9259DFBC-D495-B44E-BE0B-197FFC43B4CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="bom" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,24 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{6ED4D646-BF17-F946-8088-5887165046F1}" name="bom" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/markuslang/Desktop/suunnattava-suuntamikrofoni/pcb/ESP-32-DSP_board/production/ESP-32-DSP_board_2023-11-02_17-12-07/bom.csv" decimal="," thousands=" " comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>Designator</t>
   </si>
@@ -352,6 +333,9 @@
   </si>
   <si>
     <t>https://www.digikey.fi/fi/products/detail/samsung-electro-mechanics/CL10A105KA8NNNC/3886760</t>
+  </si>
+  <si>
+    <t>Board cost:</t>
   </si>
 </sst>
 </file>
@@ -417,8 +401,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="bom" connectionId="1" xr16:uid="{CE316101-A2CE-9A4F-8B79-30754519A974}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4DEDAF8-E664-2949-B893-5487B2DFCA60}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
+  <autoFilter ref="A1:F29" xr:uid="{A4DEDAF8-E664-2949-B893-5487B2DFCA60}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3F82D326-90B9-4849-A03D-7BEF50FD6A5B}" name="Designator"/>
+    <tableColumn id="2" xr3:uid="{68314917-E0A5-CD47-9286-CF3E62496BDE}" name="Footprint"/>
+    <tableColumn id="3" xr3:uid="{06292E2A-A947-F047-9880-A991411AB57B}" name="Quantity"/>
+    <tableColumn id="4" xr3:uid="{A0ABB874-77D9-0D4C-8555-6074E9F40795}" name="Value"/>
+    <tableColumn id="5" xr3:uid="{423E3858-3ECB-C645-9B5D-0B85C703D611}" name="Cost / unit [€]"/>
+    <tableColumn id="6" xr3:uid="{B0AC91BD-659E-C944-AE77-B109F3874369}" name="Order link" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -718,17 +713,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789DDA5E-B843-9F4D-A7DD-BCDEC96146DF}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="165" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="144.1640625" customWidth="1"/>
@@ -1312,6 +1307,17 @@
       </c>
       <c r="F29" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f>SUMPRODUCT(C2:C32,E2:E32)</f>
+        <v>49.559999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -1345,5 +1351,8 @@
     <hyperlink ref="F14" r:id="rId27" xr:uid="{935B0050-284A-0848-9134-49A229FCB193}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId28"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>